<commit_message>
Ran http on pis
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\Teaching\Spring 2020\CSC 591\Homeworks\HW3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radek/Documents/school/CSC591/IOT_HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696B3CF3-5FB9-EC45-87C1-3ACDEC5ABB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17100"/>
+    <workbookView xWindow="13120" yWindow="3440" windowWidth="20800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -65,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -487,11 +498,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -536,12 +556,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,53 +619,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,69 +907,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="13" width="10" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" customWidth="1"/>
+    <col min="14" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="22" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1"/>
@@ -948,45 +977,45 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+    <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -998,12 +1027,12 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1020,7 +1049,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1037,22 +1066,46 @@
       <c r="L6" s="2"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="8"/>
+      <c r="B7" s="6">
+        <v>4.5110000000000001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1.343</v>
+      </c>
+      <c r="D7" s="7">
+        <v>436.29</v>
+      </c>
+      <c r="E7" s="7">
+        <v>142.46</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5105.96</v>
+      </c>
+      <c r="G7" s="37">
+        <v>883.19</v>
+      </c>
+      <c r="H7" s="7">
+        <v>7012.14</v>
+      </c>
+      <c r="I7" s="38">
+        <v>1022.3</v>
+      </c>
+      <c r="J7" s="39">
+        <v>9.56</v>
+      </c>
+      <c r="K7" s="15">
+        <v>441.15</v>
+      </c>
+      <c r="L7" s="7">
+        <v>5106.5200000000004</v>
+      </c>
+      <c r="M7" s="8">
+        <v>7012.22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated MQTT stats file parser, updated Results File.xlsx
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radek/Documents/school/CSC591/IOT_HW2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinpahl/Documents/NCSU/Comp Sci Masters/CSC 591:791/Assignments/Assignment 1/IOT_HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86952F90-E7FD-654C-A445-5EBBE44330DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB07582-F144-7240-9665-BABDBDE137D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15680" yWindow="-26040" windowWidth="20800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8180" yWindow="10380" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -319,19 +322,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -495,15 +485,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -511,36 +492,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -548,21 +502,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -574,13 +513,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,31 +531,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,8 +558,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +883,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -922,54 +894,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="31" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="19" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1"/>
@@ -978,132 +950,180 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
+      <c r="B4" s="23">
+        <v>3.0176198963727199</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0.88701854723590701</v>
+      </c>
+      <c r="D4" s="24">
+        <v>178.10329826233399</v>
+      </c>
+      <c r="E4" s="24">
+        <v>33.119611438055003</v>
+      </c>
+      <c r="F4" s="24">
+        <v>1624.72417478068</v>
+      </c>
+      <c r="G4" s="24">
+        <v>820.59410309504005</v>
+      </c>
+      <c r="H4" s="24">
+        <v>811.87211008102702</v>
+      </c>
+      <c r="I4" s="25">
+        <v>167.52533726585</v>
+      </c>
+      <c r="J4" s="26">
+        <v>1.20999999999974</v>
+      </c>
+      <c r="K4" s="27">
+        <v>1.02620000000001</v>
+      </c>
+      <c r="L4" s="27">
+        <v>1.0240224609374999</v>
+      </c>
+      <c r="M4" s="28">
+        <v>1.0078306640624899</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="5"/>
+      <c r="B5" s="29">
+        <v>1.03959373775608</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0.293787289958928</v>
+      </c>
+      <c r="D5" s="30">
+        <v>79.943300124757499</v>
+      </c>
+      <c r="E5" s="30">
+        <v>15.188980261646799</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1517.32661261556</v>
+      </c>
+      <c r="G5" s="30">
+        <v>456.79227781619699</v>
+      </c>
+      <c r="H5" s="30">
+        <v>1928.6923804854</v>
+      </c>
+      <c r="I5" s="31">
+        <v>506.44985189132899</v>
+      </c>
+      <c r="J5" s="32">
+        <v>1.20999999999974</v>
+      </c>
+      <c r="K5" s="30">
+        <v>1.02620000000001</v>
+      </c>
+      <c r="L5" s="30">
+        <v>1.0240224609374999</v>
+      </c>
+      <c r="M5" s="31">
+        <v>1.0078306640624899</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="5"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="31"/>
     </row>
     <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="33">
         <v>10.53</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="34">
         <v>3.25</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="34">
         <v>803.85</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="34">
         <v>225.7</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="34">
         <v>5837.7</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="34">
         <v>1245.7</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="34">
         <v>5813.3</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="35">
         <v>496.3</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="36">
         <v>6.7119999999999997</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="34">
         <v>1.103</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="34">
         <v>1.046</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="35">
         <v>1.046</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HTTP update using only HTTP headers:
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radek/Documents/school/CSC591/IOT_HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86952F90-E7FD-654C-A445-5EBBE44330DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7821D7E6-B082-7545-B06E-604034D4AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15680" yWindow="-26040" windowWidth="20800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -319,19 +319,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -495,15 +482,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -511,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -526,15 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -553,16 +522,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -574,13 +540,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,40 +558,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -922,54 +879,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="31" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="19" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1"/>
@@ -978,62 +935,62 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
@@ -1044,13 +1001,13 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
@@ -1061,50 +1018,50 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="14"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
-        <v>10.53</v>
-      </c>
-      <c r="C7" s="7">
-        <v>3.25</v>
-      </c>
-      <c r="D7" s="7">
-        <v>803.85</v>
-      </c>
-      <c r="E7" s="7">
-        <v>225.7</v>
-      </c>
-      <c r="F7" s="7">
-        <v>5837.7</v>
-      </c>
-      <c r="G7" s="28">
-        <v>1245.7</v>
-      </c>
-      <c r="H7" s="7">
-        <v>5813.3</v>
-      </c>
-      <c r="I7" s="29">
-        <v>496.3</v>
-      </c>
-      <c r="J7" s="30">
-        <v>6.7119999999999997</v>
-      </c>
-      <c r="K7" s="15">
-        <v>1.103</v>
-      </c>
-      <c r="L7" s="7">
-        <v>1.046</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1.046</v>
+      <c r="B7">
+        <v>11.01</v>
+      </c>
+      <c r="C7">
+        <v>3.13</v>
+      </c>
+      <c r="D7">
+        <v>735.13</v>
+      </c>
+      <c r="E7">
+        <v>264.89999999999998</v>
+      </c>
+      <c r="F7">
+        <v>2122.27</v>
+      </c>
+      <c r="G7">
+        <v>500.15</v>
+      </c>
+      <c r="H7">
+        <v>5662.31</v>
+      </c>
+      <c r="I7">
+        <v>1622.94</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>1.02</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Results File.xlsx with final results.
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radek/Documents/school/CSC591/IOT_HW2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinpahl/Documents/NCSU/Comp Sci Masters/CSC 591:791/Assignments/Assignment 1/IOT_HW2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E767598A-5D3D-1449-8017-CA0DB777F7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAFD178-66CF-3E4B-9B5F-34F91168061F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="3400" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -309,19 +309,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -351,30 +338,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -486,13 +449,65 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,24 +528,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -540,15 +546,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -557,37 +554,61 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,7 +892,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -882,44 +903,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="24" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
@@ -962,16 +983,16 @@
       <c r="I3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="26" t="s">
         <v>4</v>
       </c>
     </row>
@@ -979,122 +1000,122 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
-        <v>3.0176198963727199</v>
-      </c>
-      <c r="C4" s="15">
-        <v>0.88701854723590701</v>
-      </c>
-      <c r="D4" s="15">
-        <v>178.10329826233399</v>
-      </c>
-      <c r="E4" s="15">
-        <v>33.119611438055003</v>
-      </c>
-      <c r="F4" s="15">
-        <v>1624.72417478068</v>
-      </c>
-      <c r="G4" s="15">
-        <v>820.59410309504005</v>
-      </c>
-      <c r="H4" s="15">
-        <v>811.87211008102702</v>
-      </c>
-      <c r="I4" s="16">
-        <v>167.52533726585</v>
-      </c>
-      <c r="J4" s="17">
-        <v>1.20999999999974</v>
-      </c>
-      <c r="K4" s="18">
-        <v>1.02620000000001</v>
-      </c>
-      <c r="L4" s="18">
-        <v>1.0240224609374999</v>
-      </c>
-      <c r="M4" s="19">
-        <v>1.0078306640624899</v>
+      <c r="B4" s="30">
+        <v>25.012</v>
+      </c>
+      <c r="C4" s="31">
+        <v>5.8810000000000002</v>
+      </c>
+      <c r="D4" s="31">
+        <v>1678.241</v>
+      </c>
+      <c r="E4" s="31">
+        <v>354.197</v>
+      </c>
+      <c r="F4" s="31">
+        <v>9284.7860000000001</v>
+      </c>
+      <c r="G4" s="31">
+        <v>5002.826</v>
+      </c>
+      <c r="H4" s="31">
+        <v>10936.918</v>
+      </c>
+      <c r="I4" s="36">
+        <v>1687.884</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1.21</v>
+      </c>
+      <c r="K4" s="12">
+        <v>1.002</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20">
-        <v>1.03959373775608</v>
-      </c>
-      <c r="C5" s="21">
-        <v>0.293787289958928</v>
-      </c>
-      <c r="D5" s="21">
-        <v>79.943300124757499</v>
-      </c>
-      <c r="E5" s="21">
-        <v>15.188980261646799</v>
-      </c>
-      <c r="F5" s="21">
-        <v>1517.32661261556</v>
-      </c>
-      <c r="G5" s="21">
-        <v>456.79227781619699</v>
-      </c>
-      <c r="H5" s="21">
-        <v>1928.6923804854</v>
-      </c>
-      <c r="I5" s="22">
-        <v>506.44985189132899</v>
-      </c>
-      <c r="J5" s="23">
-        <v>1.20999999999974</v>
-      </c>
-      <c r="K5" s="21">
-        <v>1.02620000000001</v>
-      </c>
-      <c r="L5" s="21">
-        <v>1.0240224609374999</v>
-      </c>
-      <c r="M5" s="22">
-        <v>1.0078306640624899</v>
+      <c r="B5" s="32">
+        <v>10.614000000000001</v>
+      </c>
+      <c r="C5" s="33">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="D5" s="33">
+        <v>854.08299999999997</v>
+      </c>
+      <c r="E5" s="33">
+        <v>142.21</v>
+      </c>
+      <c r="F5" s="33">
+        <v>10468.812</v>
+      </c>
+      <c r="G5" s="33">
+        <v>5795.991</v>
+      </c>
+      <c r="H5" s="33">
+        <v>12661.159</v>
+      </c>
+      <c r="I5" s="37">
+        <v>2413.8139999999999</v>
+      </c>
+      <c r="J5" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="K5" s="15">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="L5" s="15">
+        <v>1</v>
+      </c>
+      <c r="M5" s="16">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="20">
-        <v>113.2</v>
-      </c>
-      <c r="C6" s="21">
-        <v>19.8</v>
-      </c>
-      <c r="D6" s="21">
-        <v>677.3</v>
-      </c>
-      <c r="E6" s="21">
-        <v>128</v>
-      </c>
-      <c r="F6" s="21">
-        <v>278.89999999999998</v>
-      </c>
-      <c r="G6" s="21">
-        <v>52.2</v>
-      </c>
-      <c r="H6" s="21">
-        <v>209.9</v>
-      </c>
-      <c r="I6" s="22">
-        <v>5.5</v>
-      </c>
-      <c r="J6" s="23">
+      <c r="B6" s="32">
+        <v>77.260000000000005</v>
+      </c>
+      <c r="C6" s="33">
+        <v>16.43</v>
+      </c>
+      <c r="D6" s="33">
+        <v>604.71</v>
+      </c>
+      <c r="E6" s="33">
+        <v>96.24</v>
+      </c>
+      <c r="F6" s="33">
+        <v>717.3</v>
+      </c>
+      <c r="G6" s="33">
+        <v>50.07</v>
+      </c>
+      <c r="H6" s="33">
+        <v>547.03</v>
+      </c>
+      <c r="I6" s="37">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="J6" s="14">
         <v>1.07</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="15">
         <v>1.01</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="15">
         <v>1.0109999999999999</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="16">
         <v>1.0109999999999999</v>
       </c>
     </row>
@@ -1102,40 +1123,40 @@
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>10.75</v>
-      </c>
-      <c r="C7">
-        <v>3.06</v>
-      </c>
-      <c r="D7">
-        <v>717.9</v>
-      </c>
-      <c r="E7">
-        <v>258.7</v>
-      </c>
-      <c r="F7">
-        <v>2072.5</v>
-      </c>
-      <c r="G7">
-        <v>488.4</v>
-      </c>
-      <c r="H7">
-        <v>5529.6</v>
-      </c>
-      <c r="I7">
-        <v>1584.9</v>
-      </c>
-      <c r="J7">
+      <c r="B7" s="34">
+        <v>77.55</v>
+      </c>
+      <c r="C7" s="35">
+        <v>21.24</v>
+      </c>
+      <c r="D7" s="35">
+        <v>7111.16</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1092.0999999999999</v>
+      </c>
+      <c r="F7" s="35">
+        <v>33722.129999999997</v>
+      </c>
+      <c r="G7" s="35">
+        <v>9770.02</v>
+      </c>
+      <c r="H7" s="35">
+        <v>65325.11</v>
+      </c>
+      <c r="I7" s="38">
+        <v>9989.85</v>
+      </c>
+      <c r="J7" s="29">
         <v>3</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="27">
         <v>1.02</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="27">
         <v>1</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="28">
         <v>1</v>
       </c>
     </row>

</xml_diff>